<commit_message>
desarrollando dovolucion y autenticacion login
</commit_message>
<xml_diff>
--- a/Codigo de Errores.xlsx
+++ b/Codigo de Errores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\PROYECTO\DESK\Api.COVENTAF\coventaf_desk4_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4136572-FF0E-4571-816A-0F2EA26D8E17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DFDD70-976A-4BF5-B479-EE485194938C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{18CCED97-19A6-46A6-8CF9-2D0117464EFA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>codigo del Error</t>
   </si>
@@ -49,6 +49,21 @@
   </si>
   <si>
     <t>SD0903231721</t>
+  </si>
+  <si>
+    <t>SL1003231009</t>
+  </si>
+  <si>
+    <t>SL1003231015</t>
+  </si>
+  <si>
+    <t>ServiceLogIn</t>
+  </si>
+  <si>
+    <t>SL1003231035</t>
+  </si>
+  <si>
+    <t>SL1003231113</t>
   </si>
 </sst>
 </file>
@@ -400,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C362114A-CBE6-477E-919C-CB85B2ED5C38}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,6 +471,38 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>